<commit_message>
Embedded and Linux added to shedule
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t xml:space="preserve">S.NO </t>
   </si>
@@ -158,15 +158,46 @@
   </si>
   <si>
     <t xml:space="preserve">Bitwise Operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lpc2148-Block diagram and Pin Configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Pins and Registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED,Switch,Buzzer Interfacing,Seven segment display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC,DC motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay,LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.Mar.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open,write,close,System calls</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -206,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -221,6 +252,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -247,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,6 +324,46 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -305,24 +383,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,6 +691,177 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
+    </row>
+    <row r="15" s="11" customFormat="true" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" s="16" customFormat="true" ht="23.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14" t="n">
+        <v>43173</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="17" t="n">
+        <v>43174</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" s="16" customFormat="true" ht="23.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="14" t="n">
+        <v>43175</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="17" t="n">
+        <v>43176</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="17" t="n">
+        <v>43177</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="17" t="n">
+        <v>43178</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" s="17" t="n">
+        <v>43179</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" s="17" t="n">
+        <v>43180</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="19"/>
+    </row>
+    <row r="29" s="5" customFormat="true" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>